<commit_message>
added description to graphs
</commit_message>
<xml_diff>
--- a/sorter_analysis.xlsx
+++ b/sorter_analysis.xlsx
@@ -276,12 +276,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -300,9 +294,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -312,17 +303,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -332,6 +323,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -681,11 +681,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="37953920"/>
-        <c:axId val="37952128"/>
+        <c:axId val="76760576"/>
+        <c:axId val="76762496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="37953920"/>
+        <c:axId val="76760576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5000"/>
@@ -716,12 +716,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37952128"/>
+        <c:crossAx val="76762496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="37952128"/>
+        <c:axId val="76762496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -764,7 +764,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37953920"/>
+        <c:crossAx val="76760576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1133,11 +1133,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="55178368"/>
-        <c:axId val="55180672"/>
+        <c:axId val="78321152"/>
+        <c:axId val="78323072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55178368"/>
+        <c:axId val="78321152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5000"/>
@@ -1168,12 +1168,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55180672"/>
+        <c:crossAx val="78323072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55180672"/>
+        <c:axId val="78323072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1216,7 +1216,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55178368"/>
+        <c:crossAx val="78321152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1585,11 +1585,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84626816"/>
-        <c:axId val="125707392"/>
+        <c:axId val="78353920"/>
+        <c:axId val="78355840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84626816"/>
+        <c:axId val="78353920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5000"/>
@@ -1620,12 +1620,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125707392"/>
+        <c:crossAx val="78355840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125707392"/>
+        <c:axId val="78355840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1668,7 +1668,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84626816"/>
+        <c:crossAx val="78353920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1799,6 +1799,99 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>178594</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>11906</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="8106322" cy="741229"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="4 CuadroTexto"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7453313" y="750094"/>
+          <a:ext cx="8106322" cy="741229"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Analizando</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> los graficos de los distintos sorters podemos  ver que estos son de orden  n^2 dado que estos crecen de manera</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>cuadratica. Esto es acuerdo a el analisis teorico de los algoritmos (dado que  tenemos un  for lineal adentro de otro for lineal).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>En el caso del insertion sorter, para el mejor caso  vemos que es de orden lineal a diferencia del  orden cuadratico que nos da </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>el analisis teorico. </a:t>
+          </a:r>
+          <a:endParaRPr lang="es-AR" sz="1100">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2091,7 +2184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
@@ -2102,418 +2195,418 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="21"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="11" t="s">
+      <c r="C3" s="20"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="3" t="s">
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="4"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="21"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
-      <c r="B4" s="12" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
+      <c r="A5" s="5">
         <v>10</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="11">
         <v>0</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="12">
         <v>1</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="13">
         <f>AVERAGE(B5:C5)</f>
         <v>0.5</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="11">
         <v>0</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="12">
         <v>0</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="13">
         <f>AVERAGE(E5:F5)</f>
         <v>0</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="11">
         <v>0</v>
       </c>
-      <c r="I5" s="17">
+      <c r="I5" s="12">
         <v>0</v>
       </c>
-      <c r="J5" s="18">
+      <c r="J5" s="13">
         <f>AVERAGE(H5:I5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
+      <c r="A6" s="5">
         <v>50</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="10">
         <v>1</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>2</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="4">
         <f t="shared" ref="D6:D14" si="0">AVERAGE(B6:C6)</f>
         <v>1.5</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="10">
         <v>0</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="3">
         <v>1</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="4">
         <f t="shared" ref="G6:G14" si="1">AVERAGE(E6:F6)</f>
         <v>0.5</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="10">
         <v>0</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="3">
         <v>0</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="4">
         <f t="shared" ref="J6:J14" si="2">AVERAGE(H6:I6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
+      <c r="A7" s="5">
         <v>100</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="10">
         <v>1</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="3">
         <v>3</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="4">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="10">
         <v>0</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="3">
         <v>0</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="10">
         <v>0</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="3">
         <v>1</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="4">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
+      <c r="A8" s="5">
         <v>250</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="10">
         <v>1</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="3">
         <v>6</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="4">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="10">
         <v>0</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="3">
         <v>3</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="4">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="10">
         <v>1</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="3">
         <v>2</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="4">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
+      <c r="A9" s="5">
         <v>500</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="10">
         <v>3</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="3">
         <v>11</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="10">
         <v>0</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="3">
         <v>7</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="4">
         <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="10">
         <v>4</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="3">
         <v>4</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="4">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
+      <c r="A10" s="5">
         <v>1000</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="10">
         <v>13</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="3">
         <v>29</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="4">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="10">
         <v>0</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="3">
         <v>25</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="4">
         <f t="shared" si="1"/>
         <v>12.5</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="10">
         <v>13</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="3">
         <v>13</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="4">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
+      <c r="A11" s="5">
         <v>2000</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="10">
         <v>45</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="3">
         <v>100</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="4">
         <f t="shared" si="0"/>
         <v>72.5</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="10">
         <v>0</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="3">
         <v>97</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="4">
         <f t="shared" si="1"/>
         <v>48.5</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11" s="10">
         <v>48</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="3">
         <v>47</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="4">
         <f t="shared" si="2"/>
         <v>47.5</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
+      <c r="A12" s="5">
         <v>3000</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="10">
         <v>105</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="3">
         <v>215</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="4">
         <f t="shared" si="0"/>
         <v>160</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="10">
         <v>0</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="3">
         <v>217</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="4">
         <f t="shared" si="1"/>
         <v>108.5</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="10">
         <v>112</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="3">
         <v>128</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="4">
         <f t="shared" si="2"/>
         <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="7">
+      <c r="A13" s="5">
         <v>4000</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="10">
         <v>182</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="3">
         <v>400</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="4">
         <f t="shared" si="0"/>
         <v>291</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="10">
         <v>0</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="3">
         <v>386</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="4">
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="10">
         <v>183</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="3">
         <v>181</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="4">
         <f t="shared" si="2"/>
         <v>182</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="8">
+      <c r="A14" s="6">
         <v>5000</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="9">
         <v>273</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="7">
         <v>592</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="8">
         <f t="shared" si="0"/>
         <v>432.5</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="9">
         <v>0</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="7">
         <v>584</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="8">
         <f t="shared" si="1"/>
         <v>292</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="9">
         <v>272</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I14" s="7">
         <v>277</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="8">
         <f t="shared" si="2"/>
         <v>274.5</v>
       </c>

</xml_diff>

<commit_message>
Corrected QuickSorter.java, added new tests to Tester.java, performed efficiency analysis on ShellSort for different H sequences
</commit_message>
<xml_diff>
--- a/sorter_analysis.xlsx
+++ b/sorter_analysis.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="14115" windowHeight="4680"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="14115" windowHeight="4680" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Bubble - Insertion - Selection" sheetId="1" r:id="rId1"/>
+    <sheet name="Shell" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>n</t>
   </si>
@@ -59,12 +59,47 @@
       <t>Resultados empiricos</t>
     </r>
   </si>
+  <si>
+    <t>Secuencia 1</t>
+  </si>
+  <si>
+    <t>Secuencia 2</t>
+  </si>
+  <si>
+    <t>Ascendente</t>
+  </si>
+  <si>
+    <t>Descencente</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Tabla 2: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Comparacion de distinas secuencias de H para el ShellSort</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,8 +133,31 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -109,6 +167,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -268,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -333,6 +397,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,7 +471,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$B$3</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -407,7 +482,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$A$5:$A$14</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$A$5:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -446,7 +521,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$B$5:$B$14</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$B$5:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -490,7 +565,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$E$3</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -501,7 +576,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$A$5:$A$14</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$A$5:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -540,7 +615,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$E$5:$E$14</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$E$5:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -584,7 +659,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$H$3</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$H$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -595,7 +670,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$A$5:$A$14</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$A$5:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -634,7 +709,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$H$5:$H$14</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$H$5:$H$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -681,11 +756,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="76760576"/>
-        <c:axId val="76762496"/>
+        <c:axId val="85431040"/>
+        <c:axId val="85432960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="76760576"/>
+        <c:axId val="85431040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5000"/>
@@ -716,12 +791,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76762496"/>
+        <c:crossAx val="85432960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76762496"/>
+        <c:axId val="85432960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -764,7 +839,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76760576"/>
+        <c:crossAx val="85431040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -848,7 +923,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$B$3</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -859,7 +934,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$A$5:$A$14</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$A$5:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -898,7 +973,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$C$5:$C$14</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$C$5:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -942,7 +1017,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$E$3</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -953,7 +1028,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$A$5:$A$14</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$A$5:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -992,7 +1067,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$F$5:$F$14</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$F$5:$F$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1036,7 +1111,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$H$3</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$H$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1047,7 +1122,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$A$5:$A$14</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$A$5:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1086,7 +1161,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$I$5:$I$14</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$I$5:$I$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1133,11 +1208,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="78321152"/>
-        <c:axId val="78323072"/>
+        <c:axId val="87257856"/>
+        <c:axId val="87259776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="78321152"/>
+        <c:axId val="87257856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5000"/>
@@ -1168,12 +1243,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78323072"/>
+        <c:crossAx val="87259776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="78323072"/>
+        <c:axId val="87259776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1216,7 +1291,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78321152"/>
+        <c:crossAx val="87257856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1300,7 +1375,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$B$3</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1311,7 +1386,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$A$5:$A$14</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$A$5:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1350,7 +1425,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$D$5:$D$14</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$D$5:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1394,7 +1469,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$E$3</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1405,7 +1480,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$A$5:$A$14</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$A$5:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1444,7 +1519,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$G$5:$G$14</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$G$5:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1488,7 +1563,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$H$3</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$H$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1499,7 +1574,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$A$5:$A$14</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$A$5:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1538,7 +1613,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$J$5:$J$14</c:f>
+              <c:f>'Bubble - Insertion - Selection'!$J$5:$J$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1585,11 +1660,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="78353920"/>
-        <c:axId val="78355840"/>
+        <c:axId val="87302912"/>
+        <c:axId val="87304832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="78353920"/>
+        <c:axId val="87302912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5000"/>
@@ -1620,12 +1695,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78355840"/>
+        <c:crossAx val="87304832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="78355840"/>
+        <c:axId val="87304832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1668,7 +1743,304 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78353920"/>
+        <c:crossAx val="87302912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="es-AR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-AR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-AR"/>
+              <a:t>Caso</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-AR" baseline="0"/>
+              <a:t> promedio</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Shell!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Secuencia 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Shell!$A$8:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Shell!$D$8:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10541.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Shell!$E$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Secuencia 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Shell!$A$8:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Shell!$G$8:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>111.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10416.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="61668736"/>
+        <c:axId val="81876480"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="61668736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Cantidad de datos</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="81876480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="81876480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="11000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Tiempo</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-AR" baseline="0"/>
+                  <a:t> (milis)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-AR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.2222222222222223E-2"/>
+              <c:y val="0.50162037037037033"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="61668736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1801,12 +2173,12 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>178594</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>11906</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>583406</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="8106322" cy="741229"/>
+    <xdr:ext cx="8106322" cy="833437"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="5" name="4 CuadroTexto"/>
@@ -1814,8 +2186,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7453313" y="750094"/>
-          <a:ext cx="8106322" cy="741229"/>
+          <a:off x="7096125" y="2821781"/>
+          <a:ext cx="8106322" cy="833437"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1838,7 +2210,7 @@
       </xdr:style>
       <xdr:txBody>
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
+          <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
@@ -1895,8 +2267,131 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>201083</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>84666</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>21166</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>140626</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="1 Gráfico"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>370417</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>169333</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5126275" cy="1125693"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="370417" y="2645833"/>
+          <a:ext cx="5126275" cy="1125693"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>Como se puede ver en el grafico</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
+            <a:t> y en la tabla, la secuencia 2 es mas rapida</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
+            <a:t>que la secuencia 1. Sin embrago esta diferencia es muy pequeña y no demuestra</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
+            <a:t>grandes ventajas de la secuencia 2 sobre la 1, comprobando de esta manera que </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
+            <a:t>la secuencia de Hs que se tome no producira grandes variaciones en la eficiencia</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
+            <a:t>del ShellSort, almenos que se tomen casos extremos como H = 1 o una variacion de Hs</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
+            <a:t>minima.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2184,11 +2679,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="11.42578125" style="1"/>
@@ -2630,13 +3125,359 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>8</v>
+      </c>
+      <c r="D1">
+        <v>23</v>
+      </c>
+      <c r="E1">
+        <v>77</v>
+      </c>
+      <c r="F1">
+        <v>281</v>
+      </c>
+      <c r="G1">
+        <v>1073</v>
+      </c>
+      <c r="H1">
+        <v>4193</v>
+      </c>
+      <c r="I1">
+        <v>16577</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>40</v>
+      </c>
+      <c r="F2">
+        <v>121</v>
+      </c>
+      <c r="G2">
+        <v>364</v>
+      </c>
+      <c r="H2">
+        <v>1093</v>
+      </c>
+      <c r="I2">
+        <v>3280</v>
+      </c>
+      <c r="J2">
+        <v>9841</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="23"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>10</v>
+      </c>
+      <c r="B8" s="11">
+        <v>1</v>
+      </c>
+      <c r="C8" s="12">
+        <v>0</v>
+      </c>
+      <c r="D8" s="13">
+        <f>AVERAGE(B8:C8)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="12">
+        <v>1</v>
+      </c>
+      <c r="F8" s="12">
+        <v>0</v>
+      </c>
+      <c r="G8" s="12">
+        <f>AVERAGE(E8:F8)</f>
+        <v>0.5</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <f>A8*10</f>
+        <v>100</v>
+      </c>
+      <c r="B9" s="10">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>6</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" ref="D9:D12" si="0">AVERAGE(B9:C9)</f>
+        <v>3</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>6</v>
+      </c>
+      <c r="G9" s="3">
+        <f>AVERAGE(E9:F9)</f>
+        <v>3</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <f t="shared" ref="A10:A11" si="1">A9*10</f>
+        <v>1000</v>
+      </c>
+      <c r="B10" s="10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <v>35</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>36</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" ref="G10:G12" si="2">AVERAGE(E10:F10)</f>
+        <v>18</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+      <c r="B11" s="10">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
+        <v>213</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" si="0"/>
+        <v>107</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
+        <v>222</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" si="2"/>
+        <v>111.5</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <f>A11*10</f>
+        <v>100000</v>
+      </c>
+      <c r="B12" s="10">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
+        <v>21082</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" si="0"/>
+        <v>10541.5</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
+        <v>20832</v>
+      </c>
+      <c r="G12" s="3">
+        <f t="shared" si="2"/>
+        <v>10416.5</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="24"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="24"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="24"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="A4:G4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="D8:D9 D10:D11 D12" formulaRange="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2646,7 +3487,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>